<commit_message>
Removed TreeServerGeoObject, LeafServerGeoObject and all dependencies on that data
</commit_message>
<xml_diff>
--- a/georegistry-test/src/test/resources/test-spreadsheet2.xlsx
+++ b/georegistry-test/src/test/resources/test-spreadsheet2.xlsx
@@ -73,7 +73,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="MM/DD/YY"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
   <fonts count="4">
@@ -156,32 +156,30 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.7"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>